<commit_message>
Added query for preference API
</commit_message>
<xml_diff>
--- a/Api_issues_list.xlsx
+++ b/Api_issues_list.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/socrates/Development/banking-app-stubs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mckinsey\codebase\banking-app-stubs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="636" yWindow="1176" windowWidth="28164" windowHeight="16884" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,8 +23,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Pawan Jashnani</author>
+  </authors>
+  <commentList>
+    <comment ref="E22" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Pawan Jashnani:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+i</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
   <si>
     <t>Stream</t>
   </si>
@@ -164,18 +198,44 @@
   <si>
     <t>There is no image url tag available for banks</t>
   </si>
+  <si>
+    <t>Make a payment- Once off - Enter amount</t>
+  </si>
+  <si>
+    <t>Preference.yaml</t>
+  </si>
+  <si>
+    <t>limits</t>
+  </si>
+  <si>
+    <t>1. How to calculate instant payment charges for specific payment.
+2. How the daily payment limit will be set. (Whether it is selected account level or user profile dependent)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -220,6 +280,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -487,24 +550,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="2" width="26.5" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="3" max="3" width="30.69921875" customWidth="1"/>
     <col min="4" max="4" width="8.5" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="61.6640625" customWidth="1"/>
+    <col min="6" max="6" width="61.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -524,7 +587,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -544,7 +607,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -564,7 +627,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -584,7 +647,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -595,28 +658,28 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -636,7 +699,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
         <v>30</v>
       </c>
@@ -650,7 +713,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="224" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="234" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -664,7 +727,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -678,7 +741,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -698,7 +761,28 @@
         <v>43</v>
       </c>
     </row>
+    <row r="22" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Api Queries for PFM Added.
</commit_message>
<xml_diff>
--- a/Api_issues_list.xlsx
+++ b/Api_issues_list.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mckinsey\codebase\banking-app-stubs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mckinseyProjects\banking-app-stubs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
   <si>
     <t>Stream</t>
   </si>
@@ -210,6 +210,21 @@
   <si>
     <t>1. How to calculate instant payment charges for specific payment.
 2. How the daily payment limit will be set. (Whether it is selected account level or user profile dependent)</t>
+  </si>
+  <si>
+    <t>PFM</t>
+  </si>
+  <si>
+    <t>Transaction Details</t>
+  </si>
+  <si>
+    <t>SCPAccounts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/scp/account/transactions </t>
+  </si>
+  <si>
+    <t>ChildTransactiosns are what   basis for the API:- account/transactions in SCPAccounts.yaml</t>
   </si>
 </sst>
 </file>
@@ -551,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -781,6 +796,36 @@
         <v>47</v>
       </c>
     </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" t="s">
+        <v>51</v>
+      </c>
+      <c r="F23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Adding some Yoddle related API Questions.
</commit_message>
<xml_diff>
--- a/Api_issues_list.xlsx
+++ b/Api_issues_list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mckinseyProjects\banking-app-stubs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mckinsey\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
   <si>
     <t>Stream</t>
   </si>
@@ -225,6 +225,27 @@
   </si>
   <si>
     <t>ChildTransactiosns are what   basis for the API:- account/transactions in SCPAccounts.yaml</t>
+  </si>
+  <si>
+    <t>Finance and Category Screen</t>
+  </si>
+  <si>
+    <t>Yoddle</t>
+  </si>
+  <si>
+    <t>What all endpoints we will be using for Income and expense for a category?</t>
+  </si>
+  <si>
+    <t>Category Secreen</t>
+  </si>
+  <si>
+    <t>What all endpoints we will be using for first level category on category Screen</t>
+  </si>
+  <si>
+    <t>Transaction</t>
+  </si>
+  <si>
+    <t>What all endpoints we will be using for second level category on category Screen</t>
   </si>
 </sst>
 </file>
@@ -566,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -579,7 +600,7 @@
     <col min="3" max="3" width="30.69921875" customWidth="1"/>
     <col min="4" max="4" width="8.5" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="61.69921875" customWidth="1"/>
+    <col min="6" max="6" width="77.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -820,10 +841,42 @@
       <c r="A24" t="s">
         <v>48</v>
       </c>
+      <c r="B24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" t="s">
+        <v>54</v>
+      </c>
+      <c r="F24" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>48</v>
+      </c>
+      <c r="B25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" t="s">
+        <v>54</v>
+      </c>
+      <c r="F25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" t="s">
+        <v>54</v>
+      </c>
+      <c r="F26" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>